<commit_message>
fix issue with units to include $ symbol in spreadsheet rather than code
</commit_message>
<xml_diff>
--- a/data/sampling/units.xlsx
+++ b/data/sampling/units.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic1901_deep_layering/github/data/sampling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7288346-6A59-2A42-B19D-B7E09CEB0494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7B1735-5885-4944-98FB-C1ED61857BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="760" windowWidth="29220" windowHeight="18880" xr2:uid="{1EDB8023-74AD-8E40-8F17-4D0EA63C8EF6}"/>
   </bookViews>
@@ -47,33 +47,18 @@
     <t>latex_name</t>
   </si>
   <si>
-    <t>\delta ^{18}O</t>
-  </si>
-  <si>
     <t>d18O</t>
   </si>
   <si>
     <t>dD</t>
   </si>
   <si>
-    <t>\delta D</t>
-  </si>
-  <si>
     <t>dxs</t>
   </si>
   <si>
-    <t>d _{xs}</t>
-  </si>
-  <si>
-    <t>CO_{2}</t>
-  </si>
-  <si>
     <t>ppm</t>
   </si>
   <si>
-    <t>CH_{4}</t>
-  </si>
-  <si>
     <t>ppb</t>
   </si>
   <si>
@@ -84,6 +69,21 @@
   </si>
   <si>
     <t>‰</t>
+  </si>
+  <si>
+    <t>$\delta ^{18}$O</t>
+  </si>
+  <si>
+    <t>$\delta$ D</t>
+  </si>
+  <si>
+    <t>d$_{xs}$</t>
+  </si>
+  <si>
+    <t>CO$_{2}$</t>
+  </si>
+  <si>
+    <t>CH$_{4}$</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,57 +476,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working context plot with extenrnal data
</commit_message>
<xml_diff>
--- a/data/sampling/units.xlsx
+++ b/data/sampling/units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic1901_deep_layering/github/data/sampling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6AB587-8807-D743-B847-6F2444857845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395348E7-0A7B-D34B-9BAA-90EF52DD82AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="760" windowWidth="29220" windowHeight="18880" xr2:uid="{1EDB8023-74AD-8E40-8F17-4D0EA63C8EF6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>simple_name</t>
   </si>
@@ -84,6 +84,30 @@
   </si>
   <si>
     <t>CH$_{4}$</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Ar Age</t>
+  </si>
+  <si>
+    <t>kyr</t>
+  </si>
+  <si>
+    <t>concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Particle Concentration </t>
+  </si>
+  <si>
+    <t>tac</t>
+  </si>
+  <si>
+    <t>Total Air Content</t>
+  </si>
+  <si>
+    <t>cm$^3$/g</t>
   </si>
 </sst>
 </file>
@@ -455,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA282E54-A88C-8E4B-A9AB-DECBBDBF30F2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,6 +553,39 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>